<commit_message>
add graphs to specific dépenses
</commit_message>
<xml_diff>
--- a/data/sorties/salaires.xlsx
+++ b/data/sorties/salaires.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
         <v>500</v>
       </c>
       <c r="D2" t="n">
-        <v>1500</v>
+        <v>-1500</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         <v>204</v>
       </c>
       <c r="D3" t="n">
-        <v>704</v>
+        <v>-704</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,39 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>400</v>
+        <v>-400</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jeanno</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Thai Nhien</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>